<commit_message>
report - add graph
</commit_message>
<xml_diff>
--- a/tts2/results.xlsx
+++ b/tts2/results.xlsx
@@ -2,22 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Users\Chase Stevens\Documents\GitHub\ttds\tts2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14925" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId3"/>
+    <pivotCache cacheId="21" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>brute.py</t>
   </si>
@@ -42,6 +44,12 @@
     <t>Grand Total</t>
   </si>
   <si>
+    <t>Sum of brute.py</t>
+  </si>
+  <si>
+    <t>Sum of index.py</t>
+  </si>
+  <si>
     <t>Row Labels</t>
   </si>
   <si>
@@ -52,6 +60,33 @@
   </si>
   <si>
     <t>best.py</t>
+  </si>
+  <si>
+    <t>Sum of best.py</t>
+  </si>
+  <si>
+    <t>no id check</t>
+  </si>
+  <si>
+    <t>tuple(tokens)</t>
+  </si>
+  <si>
+    <t>first 40 tokens</t>
+  </si>
+  <si>
+    <t>stopwords</t>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>no stoprem</t>
+  </si>
+  <si>
+    <t>best</t>
   </si>
 </sst>
 </file>
@@ -125,7 +160,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[results.xlsx]Sheet3!PivotTable2</c:name>
+    <c:name>[results.xlsx]Sheet4!PivotTable3</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -143,8 +178,8 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="triangle"/>
-          <c:size val="7"/>
+          <c:symbol val="circle"/>
+          <c:size val="5"/>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -152,33 +187,6 @@
             <a:ln w="9525">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:ln w="28575" cap="rnd">
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="7"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst/>
@@ -196,11 +204,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$B$1</c:f>
+              <c:f>Sheet4!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>brute</c:v>
+                  <c:v>Sum of brute.py</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -215,8 +223,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="7"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -229,71 +237,61 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:f>Sheet4!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2500</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$8</c:f>
+              <c:f>Sheet4!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>3.15E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.9800000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.27</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.86</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>5.14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.97</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,11 +303,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$C$1</c:f>
+              <c:f>Sheet4!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>index</c:v>
+                  <c:v>Sum of index.py</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -325,7 +323,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="7"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -338,71 +336,160 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
-            <c:forward val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet3!$A$2:$A$8</c:f>
+              <c:f>Sheet4!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2500</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5000</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>15000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$8</c:f>
+              <c:f>Sheet4!$C$2:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>3.0699999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>3.8500000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.38</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet4!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sum of best.py</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet4!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.45</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.36</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.57</c:v>
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet4!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3700000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -419,11 +506,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="400573344"/>
-        <c:axId val="400574128"/>
+        <c:axId val="400573736"/>
+        <c:axId val="400569032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="400573344"/>
+        <c:axId val="400573736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -466,7 +553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400574128"/>
+        <c:crossAx val="400569032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -474,8 +561,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="400574128"/>
+        <c:axId val="400569032"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -525,7 +613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="400573344"/>
+        <c:crossAx val="400573736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -539,14 +627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -625,7 +705,837 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[results.xlsx]Sheet6!PivotTable4</c:name>
+    <c:fmtId val="0"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm speed comparison</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="7"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="triangle"/>
+          <c:size val="7"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="diamond"/>
+          <c:size val="7"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>brute</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet6!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.15E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9800000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.6300000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>index</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet6!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.0699999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8500000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8000000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet6!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>best</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet6!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet6!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3700000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="409934024"/>
+        <c:axId val="409934416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="409934024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stories</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> processed</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409934416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="409934416"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Processing</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (minutes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="409934024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1168,20 +2078,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>466726</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1204,26 +2652,30 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="H. Chase Stevens" refreshedDate="41931.481604513887" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="6">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="H. Chase Stevens" refreshedDate="41931.580792245368" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="7">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:C7" sheet="Sheet1"/>
+    <worksheetSource ref="A1:D8" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields count="3">
+  <cacheFields count="4">
     <cacheField name="queries" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2500" maxValue="15000" count="6">
-        <n v="2500"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100" maxValue="10000" count="7">
+        <n v="100"/>
+        <n v="200"/>
+        <n v="500"/>
+        <n v="1000"/>
+        <n v="2000"/>
         <n v="5000"/>
-        <n v="7500"/>
         <n v="10000"/>
-        <n v="12500"/>
-        <n v="15000"/>
       </sharedItems>
     </cacheField>
     <cacheField name="brute.py" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.33" maxValue="11.44"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.15E-3" maxValue="5.14"/>
     </cacheField>
     <cacheField name="index.py" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.1" maxValue="3.57"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.0699999999999998E-3" maxValue="1.45"/>
+    </cacheField>
+    <cacheField name="best.py" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.3E-3" maxValue="0.32"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1235,62 +2687,76 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="6">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="7">
   <r>
     <x v="0"/>
-    <n v="0.33"/>
-    <n v="0.1"/>
+    <n v="3.15E-3"/>
+    <n v="3.0699999999999998E-3"/>
+    <n v="2.3E-3"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="1.27"/>
-    <n v="0.38"/>
+    <n v="4.9800000000000001E-3"/>
+    <n v="3.8500000000000001E-3"/>
+    <n v="3.3700000000000002E-3"/>
   </r>
   <r>
     <x v="2"/>
-    <n v="2.86"/>
-    <n v="0.84"/>
+    <n v="1.6799999999999999E-2"/>
+    <n v="7.6E-3"/>
+    <n v="4.8999999999999998E-3"/>
   </r>
   <r>
     <x v="3"/>
-    <n v="5.14"/>
-    <n v="1.45"/>
+    <n v="5.6300000000000003E-2"/>
+    <n v="1.9E-2"/>
+    <n v="8.3000000000000001E-3"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="7.97"/>
-    <n v="2.36"/>
+    <n v="0.222"/>
+    <n v="6.8000000000000005E-2"/>
+    <n v="0.02"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="11.44"/>
-    <n v="3.57"/>
+    <n v="1.27"/>
+    <n v="0.38"/>
+    <n v="0.08"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="5.14"/>
+    <n v="1.45"/>
+    <n v="0.32"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
-  <location ref="A1:C8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+  <location ref="A1:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
-      <items count="7">
+      <items count="8">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="7">
+  <rowItems count="8">
     <i>
       <x/>
     </i>
@@ -1309,6 +2775,9 @@
     <i>
       <x v="5"/>
     </i>
+    <i>
+      <x v="6"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1316,19 +2785,23 @@
   <colFields count="1">
     <field x="-2"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="3">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
   </colItems>
-  <dataFields count="2">
-    <dataField name="brute" fld="1" baseField="0" baseItem="0"/>
-    <dataField name="index" fld="2" baseField="0" baseItem="0"/>
+  <dataFields count="3">
+    <dataField name="Sum of brute.py" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Sum of index.py" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="Sum of best.py" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -1343,6 +2816,148 @@
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A1:D9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="brute" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="index" fld="2" baseField="0" baseItem="0"/>
+    <dataField name="best" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -1620,104 +3235,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2">
-        <v>0.33</v>
+        <v>3.15E-3</v>
       </c>
       <c r="C2" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0699999999999998E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
+        <v>200</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.9800000000000001E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.8500000000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.3700000000000002E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>500</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.222</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5000</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B7" s="2">
         <v>1.27</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C7" s="2">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>7500</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2.86</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="D7" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>10000</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B8" s="2">
         <v>5.14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C8" s="2">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>12500</v>
-      </c>
-      <c r="B6" s="2">
-        <v>7.97</v>
-      </c>
-      <c r="C6" s="2">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>15000</v>
-      </c>
-      <c r="B7" s="2">
-        <v>11.44</v>
-      </c>
-      <c r="C7" s="2">
-        <v>3.57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="D8" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="2">
-        <v>29.009999999999998</v>
-      </c>
-      <c r="C8" s="2">
-        <v>8.6999999999999993</v>
+      <c r="B9" s="2">
+        <v>6.7132299999999994</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.9315199999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.43886999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1728,15 +3381,161 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3.15E-3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.0699999999999998E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>200</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4.9800000000000001E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.8500000000000001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.3700000000000002E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>500</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <v>7.6E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>8.3000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.222</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="B8" s="2">
+        <v>5.14</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.45</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
+        <v>6.7132299999999994</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.9315199999999999</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.43886999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1747,73 +3546,316 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="B2">
-        <v>0.33</v>
+        <v>2.6099999999999999E-3</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.4399999999999999E-3</v>
+      </c>
+      <c r="D2">
+        <v>2.5200000000000001E-3</v>
+      </c>
+      <c r="F2">
+        <f>B2/C2</f>
+        <v>1.069672131147541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>200</v>
+      </c>
+      <c r="B3">
+        <v>4.1599999999999996E-3</v>
+      </c>
+      <c r="C3">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>2.63E-3</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" si="0">B3/C3</f>
+        <v>1.3081761006289307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>500</v>
+      </c>
+      <c r="B4">
+        <v>1.47E-2</v>
+      </c>
+      <c r="C4">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="D4">
+        <v>3.2100000000000002E-3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2.2615384615384615</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1000</v>
+      </c>
+      <c r="B5">
+        <v>5.04E-2</v>
+      </c>
+      <c r="C5">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>4.15E-3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>2.9647058823529409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2000</v>
+      </c>
+      <c r="B6">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="C6">
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="D6">
+        <v>6.9699999999999996E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3.4548611111111116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5000</v>
       </c>
+      <c r="B7">
+        <v>1.34</v>
+      </c>
+      <c r="C7">
+        <v>0.34</v>
+      </c>
+      <c r="D7">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>3.9411764705882351</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10000</v>
+      </c>
+      <c r="B8">
+        <v>5.4</v>
+      </c>
+      <c r="C8">
+        <v>1.41</v>
+      </c>
+      <c r="D8">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.84640000000000004</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>3.8297872340425538</v>
+      </c>
+      <c r="G8">
+        <f>B8/D8</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="H8">
+        <f>C8/D8</f>
+        <v>18.650793650793648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12500</v>
+      </c>
+      <c r="F9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>15000</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>50000</v>
+      </c>
+      <c r="D11">
+        <v>2.9220000000000002</v>
+      </c>
+      <c r="E11">
+        <v>1.7175</v>
+      </c>
+      <c r="F11">
+        <v>1.6908000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T14">
+        <f>1-0.9113</f>
+        <v>8.8700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>E8/D8</f>
+        <v>11.195767195767196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>172</v>
+      </c>
+      <c r="B2">
+        <v>90.352999999999994</v>
+      </c>
+      <c r="C2">
+        <v>1.6908000000000001</v>
+      </c>
+      <c r="D2">
+        <f>C2*60</f>
+        <v>101.44800000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>153</v>
+      </c>
       <c r="B3">
-        <v>1.27</v>
-      </c>
-      <c r="C3">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.436999999999998</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="0">C3*60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>7500</v>
+        <v>161</v>
       </c>
       <c r="B4">
-        <v>2.86</v>
-      </c>
-      <c r="C4">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.29</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>D7/D2</f>
+        <v>1.0955169150697894</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>10000</v>
+        <v>166</v>
       </c>
       <c r="B5">
-        <v>5.14</v>
-      </c>
-      <c r="C5">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90.82</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>12500</v>
+        <v>163</v>
       </c>
       <c r="B6">
-        <v>7.97</v>
-      </c>
-      <c r="C6">
-        <v>2.36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.13</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>15000</v>
+        <v>164</v>
       </c>
       <c r="B7">
-        <v>11.44</v>
+        <v>91.13</v>
       </c>
       <c r="C7">
-        <v>3.57</v>
+        <v>1.8523000000000001</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>111.13800000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f>0.9113-0.90353</f>
+        <v>7.7699999999999436E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>